<commit_message>
Revert "Merge branch 'Larry'"
This reverts commit 62422c7caff91b755184e2c2b4f405a461855ef8, reversing
changes made to c68fd995c46f872b7ab8a35acb38e40466dbe71c.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总-10.xlsx
+++ b/作业完成情况汇总-10.xlsx
@@ -229,10 +229,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -264,44 +264,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -325,13 +287,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -350,9 +305,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -373,14 +328,51 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -395,14 +387,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -429,6 +429,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -465,18 +489,114 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -490,126 +610,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -720,17 +720,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -755,6 +744,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -769,10 +769,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -781,133 +781,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="13"/>

</xml_diff>